<commit_message>
commiting processlead table is updated
</commit_message>
<xml_diff>
--- a/processlead.xlsx
+++ b/processlead.xlsx
@@ -19,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5" uniqueCount="5">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="8" uniqueCount="8">
   <si>
     <t>sl.no</t>
   </si>
@@ -27,13 +27,22 @@
     <t>date</t>
   </si>
   <si>
-    <t>Name</t>
-  </si>
-  <si>
-    <t>salary</t>
-  </si>
-  <si>
-    <t>remarks</t>
+    <t>Project reviews</t>
+  </si>
+  <si>
+    <t>Sprint1</t>
+  </si>
+  <si>
+    <t>review comments</t>
+  </si>
+  <si>
+    <t>action plan</t>
+  </si>
+  <si>
+    <t>owner</t>
+  </si>
+  <si>
+    <t>status remarks</t>
   </si>
 </sst>
 </file>
@@ -69,8 +78,9 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="15" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -351,15 +361,22 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:E1"/>
+  <dimension ref="A1:G33"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="H1" sqref="H1:H1048576"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="2" max="2" width="9.08984375" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="13.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="10" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="13.1796875" bestFit="1" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:7" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -370,10 +387,179 @@
         <v>2</v>
       </c>
       <c r="D1" t="s">
+        <v>4</v>
+      </c>
+      <c r="E1" t="s">
+        <v>5</v>
+      </c>
+      <c r="F1" t="s">
+        <v>6</v>
+      </c>
+      <c r="G1" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="2" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B2" s="1">
+        <v>45292</v>
+      </c>
+      <c r="C2" t="s">
         <v>3</v>
       </c>
-      <c r="E1" t="s">
-        <v>4</v>
+    </row>
+    <row r="3" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B3" s="1">
+        <v>45293</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B4" s="1">
+        <v>45294</v>
+      </c>
+    </row>
+    <row r="5" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B5" s="1">
+        <v>45295</v>
+      </c>
+    </row>
+    <row r="6" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B6" s="1">
+        <v>45296</v>
+      </c>
+    </row>
+    <row r="7" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B7" s="1">
+        <v>45297</v>
+      </c>
+    </row>
+    <row r="8" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B8" s="1">
+        <v>45298</v>
+      </c>
+    </row>
+    <row r="9" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B9" s="1">
+        <v>45299</v>
+      </c>
+    </row>
+    <row r="10" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B10" s="1">
+        <v>45300</v>
+      </c>
+    </row>
+    <row r="11" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B11" s="1">
+        <v>45301</v>
+      </c>
+    </row>
+    <row r="12" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B12" s="1">
+        <v>45302</v>
+      </c>
+    </row>
+    <row r="13" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B13" s="1">
+        <v>45303</v>
+      </c>
+    </row>
+    <row r="14" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B14" s="1">
+        <v>45304</v>
+      </c>
+    </row>
+    <row r="15" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B15" s="1">
+        <v>45305</v>
+      </c>
+    </row>
+    <row r="16" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B16" s="1">
+        <v>45306</v>
+      </c>
+    </row>
+    <row r="17" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B17" s="1">
+        <v>45307</v>
+      </c>
+    </row>
+    <row r="18" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B18" s="1">
+        <v>45308</v>
+      </c>
+    </row>
+    <row r="19" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B19" s="1">
+        <v>45309</v>
+      </c>
+    </row>
+    <row r="20" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B20" s="1">
+        <v>45310</v>
+      </c>
+    </row>
+    <row r="21" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B21" s="1">
+        <v>45311</v>
+      </c>
+    </row>
+    <row r="22" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B22" s="1">
+        <v>45312</v>
+      </c>
+    </row>
+    <row r="23" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B23" s="1">
+        <v>45313</v>
+      </c>
+    </row>
+    <row r="24" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B24" s="1">
+        <v>45314</v>
+      </c>
+    </row>
+    <row r="25" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B25" s="1">
+        <v>45315</v>
+      </c>
+    </row>
+    <row r="26" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B26" s="1">
+        <v>45316</v>
+      </c>
+    </row>
+    <row r="27" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B27" s="1">
+        <v>45317</v>
+      </c>
+    </row>
+    <row r="28" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B28" s="1">
+        <v>45318</v>
+      </c>
+    </row>
+    <row r="29" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B29" s="1">
+        <v>45319</v>
+      </c>
+    </row>
+    <row r="30" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B30" s="1">
+        <v>45320</v>
+      </c>
+    </row>
+    <row r="31" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B31" s="1">
+        <v>45321</v>
+      </c>
+    </row>
+    <row r="32" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B32" s="1">
+        <v>45322</v>
+      </c>
+    </row>
+    <row r="33" spans="2:2" x14ac:dyDescent="0.35">
+      <c r="B33" s="1">
+        <v>45323</v>
       </c>
     </row>
   </sheetData>

</xml_diff>